<commit_message>
Add GNL_CD-all-coded-drug.xlsx Merge GNL_CD codes with GNL_CD-all-coded-drug.xlsx Modify test data to provide COVID MID match with past data
</commit_message>
<xml_diff>
--- a/Data/HIRA COVID-19 Sample Data_20200325.xlsx
+++ b/Data/HIRA COVID-19 Sample Data_20200325.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Korea/opendata4covid19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1125F078-9363-D049-965E-56C9D7C4FFFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881C3BD0-1CC6-404F-8AB0-DD34CFBC0C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35980" windowHeight="13380" tabRatio="948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35980" windowHeight="13380" tabRatio="948" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table구성" sheetId="9" r:id="rId1"/>
@@ -2661,7 +2661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2818,7 +2818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
@@ -5021,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5962,7 +5962,7 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="10">
-        <v>11777</v>
+        <v>12340</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>32</v>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="10">
-        <v>11454</v>
+        <v>12341</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>32</v>
@@ -6186,7 +6186,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="10">
-        <v>11906</v>
+        <v>12342</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>32</v>
@@ -69244,7 +69244,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -69550,7 +69550,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="10">
-        <v>11125</v>
+        <v>12340</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>676</v>
@@ -69586,7 +69586,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="10">
-        <v>11129</v>
+        <v>12341</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>677</v>
@@ -69622,7 +69622,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="10">
-        <v>11132</v>
+        <v>12342</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>678</v>

</xml_diff>

<commit_message>
Modify sample data to test AGE_RANGE
</commit_message>
<xml_diff>
--- a/Data/HIRA COVID-19 Sample Data_20200325.xlsx
+++ b/Data/HIRA COVID-19 Sample Data_20200325.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Korea/opendata4covid19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881C3BD0-1CC6-404F-8AB0-DD34CFBC0C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9FC323-26DE-3447-BAAC-D8E569AF7282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35980" windowHeight="13380" tabRatio="948" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3400" yWindow="860" windowWidth="35980" windowHeight="13380" tabRatio="948" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table구성" sheetId="9" r:id="rId1"/>
@@ -2819,7 +2819,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2974,11 +2974,11 @@
         <v>627</v>
       </c>
       <c r="F2" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4">
         <f>F2</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3">
         <v>22221</v>
@@ -3071,11 +3071,11 @@
         <v>628</v>
       </c>
       <c r="F3" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" ref="G3:G11" si="1">F3</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3">
         <v>22221</v>
@@ -3168,11 +3168,11 @@
         <v>629</v>
       </c>
       <c r="F4" s="4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3">
         <v>22221</v>
@@ -3265,11 +3265,11 @@
         <v>630</v>
       </c>
       <c r="F5" s="4">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H5" s="3">
         <v>22221</v>
@@ -3362,11 +3362,11 @@
         <v>631</v>
       </c>
       <c r="F6" s="4">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3">
         <v>22221</v>
@@ -3459,11 +3459,11 @@
         <v>632</v>
       </c>
       <c r="F7" s="4">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H7" s="3">
         <v>22221</v>
@@ -3556,11 +3556,11 @@
         <v>633</v>
       </c>
       <c r="F8" s="4">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="H8" s="3">
         <v>22221</v>
@@ -3652,11 +3652,11 @@
         <v>634</v>
       </c>
       <c r="F9" s="4">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3">
         <v>22221</v>
@@ -3748,11 +3748,11 @@
         <v>635</v>
       </c>
       <c r="F10" s="4">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="H10" s="3">
         <v>22221</v>
@@ -3844,11 +3844,11 @@
         <v>636</v>
       </c>
       <c r="F11" s="4">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="H11" s="3">
         <v>22221</v>
@@ -5022,7 +5022,7 @@
   <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5307,11 +5307,11 @@
         <v>658</v>
       </c>
       <c r="F3" s="9">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ref="G3:G11" si="0">F3</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H3" s="10">
         <v>29586</v>
@@ -5416,11 +5416,11 @@
         <v>658</v>
       </c>
       <c r="F4" s="9">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H4" s="10">
         <v>50338</v>
@@ -5527,11 +5527,11 @@
         <v>658</v>
       </c>
       <c r="F5" s="9">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H5" s="10">
         <v>29489</v>
@@ -5640,11 +5640,11 @@
         <v>658</v>
       </c>
       <c r="F6" s="9">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H6" s="10">
         <v>44067</v>
@@ -5753,11 +5753,11 @@
         <v>658</v>
       </c>
       <c r="F7" s="9">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H7" s="10">
         <v>8812</v>
@@ -5866,11 +5866,11 @@
         <v>658</v>
       </c>
       <c r="F8" s="9">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H8" s="10">
         <v>85060</v>
@@ -5977,11 +5977,11 @@
         <v>658</v>
       </c>
       <c r="F9" s="9">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="H9" s="10">
         <v>86215</v>
@@ -6088,11 +6088,11 @@
         <v>658</v>
       </c>
       <c r="F10" s="9">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H10" s="10">
         <v>7551</v>
@@ -6201,11 +6201,11 @@
         <v>658</v>
       </c>
       <c r="F11" s="9">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="H11" s="10">
         <v>66754</v>

</xml_diff>

<commit_message>
Adjust sample data a little and add some more basic analytics
</commit_message>
<xml_diff>
--- a/Data/HIRA COVID-19 Sample Data_20200325.xlsx
+++ b/Data/HIRA COVID-19 Sample Data_20200325.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Korea/opendata4covid19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9FC323-26DE-3447-BAAC-D8E569AF7282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77528731-033D-944C-9945-C8D0CDFB22E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="860" windowWidth="35980" windowHeight="13380" tabRatio="948" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7540" yWindow="1920" windowWidth="35980" windowHeight="13380" tabRatio="948" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table구성" sheetId="9" r:id="rId1"/>
@@ -2818,8 +2818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -3136,7 +3136,7 @@
         <v>41</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>41</v>
@@ -3233,7 +3233,7 @@
         <v>41</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="AC4" s="2" t="s">
         <v>41</v>
@@ -3275,7 +3275,7 @@
         <v>22221</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>35</v>
@@ -3330,7 +3330,7 @@
         <v>41</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC5" s="2" t="s">
         <v>41</v>
@@ -5021,7 +5021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F11"/>
     </sheetView>
   </sheetViews>
@@ -69244,7 +69244,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -69334,7 +69334,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="10">
-        <v>11114</v>
+        <v>12340</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>670</v>
@@ -69370,7 +69370,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="10">
-        <v>11117</v>
+        <v>12341</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>671</v>
@@ -69406,7 +69406,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="10">
-        <v>11119</v>
+        <v>12342</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>672</v>
@@ -69442,7 +69442,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="10">
-        <v>11121</v>
+        <v>12340</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>673</v>
@@ -69478,7 +69478,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="10">
-        <v>11123</v>
+        <v>12341</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>674</v>
@@ -69514,7 +69514,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="10">
-        <v>11124</v>
+        <v>12342</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>675</v>

</xml_diff>